<commit_message>
Updated w/ US Core profile mappings
</commit_message>
<xml_diff>
--- a/HL7_Dental_Summary_Exchange_Requirements_20191016.xlsx
+++ b/HL7_Dental_Summary_Exchange_Requirements_20191016.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David deRoode\OneDrive - Lantana Consulting Group\Desktop\SourceControl\Git\HL7\CDA\Dental data exchange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="13_ncr:1_{47C6044E-907C-4994-9FAF-434AD9DB98B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F80CC558-DA5E-4D85-AA8C-68A87A012289}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="13_ncr:1_{47C6044E-907C-4994-9FAF-434AD9DB98B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A3BCB6DE-FCE1-4BF7-8EC1-D8770DE66132}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="385" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3847" uniqueCount="884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3890" uniqueCount="906">
   <si>
     <t>Section Header</t>
   </si>
@@ -3348,9 +3348,6 @@
     <t>Condition.text</t>
   </si>
   <si>
-    <t>Condition.code (1..1?)</t>
-  </si>
-  <si>
     <t>Condition.clinicalStatus</t>
   </si>
   <si>
@@ -3360,9 +3357,6 @@
     <t>Date diagnosis was first recorded by the author/source? Or ever?</t>
   </si>
   <si>
-    <t>BodyStructure?</t>
-  </si>
-  <si>
     <t>Condition.abatement[DateTime]</t>
   </si>
   <si>
@@ -3388,6 +3382,78 @@
   </si>
   <si>
     <t>Procedure.location</t>
+  </si>
+  <si>
+    <t>Patient.name</t>
+  </si>
+  <si>
+    <t>Patient.address</t>
+  </si>
+  <si>
+    <t>Patient.identifier</t>
+  </si>
+  <si>
+    <t>Patient.telecom</t>
+  </si>
+  <si>
+    <t>Patient.gender</t>
+  </si>
+  <si>
+    <t>Patient.birthDate</t>
+  </si>
+  <si>
+    <t>Patient.maritalStatus</t>
+  </si>
+  <si>
+    <t>Patient.us-core-race</t>
+  </si>
+  <si>
+    <t>Patient.us-core-ethnicity</t>
+  </si>
+  <si>
+    <t>Patient.communication.language</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-race</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-ethnicity</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/ValueSet/simple-language</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/marital-status</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/administrative-gender</t>
+  </si>
+  <si>
+    <t>AdministrativeGender</t>
+  </si>
+  <si>
+    <t>MaritalStatus</t>
+  </si>
+  <si>
+    <t>us-core-race</t>
+  </si>
+  <si>
+    <t>us-core-ethnicity</t>
+  </si>
+  <si>
+    <t>LanguageCodesWithLanguageAndOptionallyARegionModifier</t>
+  </si>
+  <si>
+    <t>Condition.code</t>
+  </si>
+  <si>
+    <t>BodyStructure</t>
+  </si>
+  <si>
+    <t>BodyStructure.extension</t>
+  </si>
+  <si>
+    <t>BodyStructure.location</t>
   </si>
 </sst>
 </file>
@@ -3398,7 +3464,7 @@
     <numFmt numFmtId="164" formatCode="mm\-dd\-yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0000000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3505,6 +3571,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -3598,12 +3678,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -3833,15 +3914,18 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="40% - Accent6" xfId="1" builtinId="51"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
@@ -11178,7 +11262,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0600-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0600-000000000000}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="13">
     <pivotField dataField="1" showAll="0"/>
@@ -12878,10 +12962,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>636</v>
       </c>
-      <c r="B1" s="87"/>
+      <c r="B1" s="88"/>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
@@ -12962,10 +13046,10 @@
       <c r="B14" s="26"/>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="87" t="s">
+      <c r="A15" s="88" t="s">
         <v>605</v>
       </c>
-      <c r="B15" s="87"/>
+      <c r="B15" s="88"/>
     </row>
     <row r="16" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
@@ -13223,9 +13307,9 @@
   </sheetPr>
   <dimension ref="A1:AB478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N100" sqref="N100"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N83" sqref="N83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13355,7 +13439,9 @@
       <c r="O2" s="15" t="s">
         <v>840</v>
       </c>
-      <c r="P2" s="15"/>
+      <c r="P2" s="15" t="s">
+        <v>882</v>
+      </c>
       <c r="Q2" s="15"/>
       <c r="R2" s="15"/>
       <c r="S2" s="15"/>
@@ -13402,7 +13488,9 @@
       <c r="O3" s="15" t="s">
         <v>840</v>
       </c>
-      <c r="P3" s="15"/>
+      <c r="P3" s="15" t="s">
+        <v>884</v>
+      </c>
       <c r="Q3" s="15"/>
       <c r="R3" s="15"/>
       <c r="S3" s="15"/>
@@ -13449,7 +13537,9 @@
       <c r="O4" s="15" t="s">
         <v>840</v>
       </c>
-      <c r="P4" s="15"/>
+      <c r="P4" s="15" t="s">
+        <v>884</v>
+      </c>
       <c r="Q4" s="15"/>
       <c r="R4" s="15"/>
       <c r="S4" s="15"/>
@@ -13496,7 +13586,9 @@
       <c r="O5" s="15" t="s">
         <v>840</v>
       </c>
-      <c r="P5" s="15"/>
+      <c r="P5" s="15" t="s">
+        <v>883</v>
+      </c>
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
       <c r="S5" s="15"/>
@@ -13543,14 +13635,16 @@
       <c r="O6" s="15" t="s">
         <v>840</v>
       </c>
-      <c r="P6" s="15"/>
+      <c r="P6" s="15" t="s">
+        <v>885</v>
+      </c>
       <c r="Q6" s="15"/>
       <c r="R6" s="15"/>
       <c r="S6" s="15"/>
       <c r="T6" s="15"/>
       <c r="U6" s="79"/>
     </row>
-    <row r="7" spans="1:21" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.15">
       <c r="A7" s="44">
         <v>6</v>
       </c>
@@ -13592,10 +13686,16 @@
       <c r="O7" s="15" t="s">
         <v>840</v>
       </c>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
+      <c r="P7" s="15" t="s">
+        <v>886</v>
+      </c>
+      <c r="Q7" s="15" t="s">
+        <v>897</v>
+      </c>
       <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
+      <c r="S7" s="90" t="s">
+        <v>896</v>
+      </c>
       <c r="T7" s="15"/>
       <c r="U7" s="79"/>
     </row>
@@ -13639,14 +13739,16 @@
       <c r="O8" s="15" t="s">
         <v>840</v>
       </c>
-      <c r="P8" s="15"/>
+      <c r="P8" s="15" t="s">
+        <v>887</v>
+      </c>
       <c r="Q8" s="15"/>
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
       <c r="T8" s="15"/>
       <c r="U8" s="79"/>
     </row>
-    <row r="9" spans="1:21" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.15">
       <c r="A9" s="44">
         <v>8</v>
       </c>
@@ -13688,10 +13790,16 @@
       <c r="O9" s="15" t="s">
         <v>840</v>
       </c>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
+      <c r="P9" s="15" t="s">
+        <v>888</v>
+      </c>
+      <c r="Q9" s="15" t="s">
+        <v>898</v>
+      </c>
       <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
+      <c r="S9" s="90" t="s">
+        <v>895</v>
+      </c>
       <c r="T9" s="15"/>
       <c r="U9" s="79"/>
     </row>
@@ -13737,10 +13845,16 @@
       <c r="O10" s="15" t="s">
         <v>840</v>
       </c>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
+      <c r="P10" s="15" t="s">
+        <v>889</v>
+      </c>
+      <c r="Q10" s="15" t="s">
+        <v>899</v>
+      </c>
       <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
+      <c r="S10" s="89" t="s">
+        <v>892</v>
+      </c>
       <c r="T10" s="15"/>
       <c r="U10" s="79"/>
     </row>
@@ -13786,14 +13900,20 @@
       <c r="O11" s="15" t="s">
         <v>840</v>
       </c>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
+      <c r="P11" s="15" t="s">
+        <v>890</v>
+      </c>
+      <c r="Q11" s="15" t="s">
+        <v>900</v>
+      </c>
       <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
+      <c r="S11" s="89" t="s">
+        <v>893</v>
+      </c>
       <c r="T11" s="15"/>
       <c r="U11" s="79"/>
     </row>
-    <row r="12" spans="1:21" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.15">
       <c r="A12" s="44">
         <v>11</v>
       </c>
@@ -13835,10 +13955,16 @@
       <c r="O12" s="15" t="s">
         <v>840</v>
       </c>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
+      <c r="P12" s="15" t="s">
+        <v>891</v>
+      </c>
+      <c r="Q12" s="90" t="s">
+        <v>901</v>
+      </c>
       <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
+      <c r="S12" s="90" t="s">
+        <v>894</v>
+      </c>
       <c r="T12" s="15"/>
       <c r="U12" s="79"/>
     </row>
@@ -15516,7 +15642,7 @@
       <c r="R48" s="79"/>
       <c r="S48" s="79"/>
     </row>
-    <row r="49" spans="1:21" s="47" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:21" s="47" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A49" s="44">
         <v>48</v>
       </c>
@@ -16085,7 +16211,7 @@
       </c>
       <c r="U59" s="80"/>
     </row>
-    <row r="60" spans="1:21" s="47" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:21" s="47" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A60" s="44">
         <v>59</v>
       </c>
@@ -16920,8 +17046,12 @@
       <c r="M77" s="15" t="s">
         <v>784</v>
       </c>
-      <c r="N77" s="15"/>
-      <c r="O77" s="15"/>
+      <c r="N77" s="15" t="s">
+        <v>866</v>
+      </c>
+      <c r="O77" s="15" t="s">
+        <v>840</v>
+      </c>
       <c r="P77" s="15" t="s">
         <v>869</v>
       </c>
@@ -16965,10 +17095,14 @@
       <c r="M78" s="15" t="s">
         <v>785</v>
       </c>
-      <c r="N78" s="15"/>
-      <c r="O78" s="15"/>
+      <c r="N78" s="15" t="s">
+        <v>866</v>
+      </c>
+      <c r="O78" s="15" t="s">
+        <v>840</v>
+      </c>
       <c r="P78" s="21" t="s">
-        <v>870</v>
+        <v>902</v>
       </c>
       <c r="Q78" s="15"/>
       <c r="R78" s="15"/>
@@ -17003,7 +17137,7 @@
       <c r="J79" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="K79" s="88" t="s">
+      <c r="K79" s="87" t="s">
         <v>744</v>
       </c>
       <c r="L79" s="15" t="s">
@@ -17012,10 +17146,14 @@
       <c r="M79" s="15" t="s">
         <v>785</v>
       </c>
-      <c r="N79" s="15"/>
-      <c r="O79" s="15"/>
+      <c r="N79" s="15" t="s">
+        <v>866</v>
+      </c>
+      <c r="O79" s="15" t="s">
+        <v>840</v>
+      </c>
       <c r="P79" s="21" t="s">
-        <v>870</v>
+        <v>902</v>
       </c>
       <c r="Q79" s="15"/>
       <c r="R79" s="15"/>
@@ -17059,10 +17197,14 @@
       <c r="M80" s="15" t="s">
         <v>785</v>
       </c>
-      <c r="N80" s="15"/>
-      <c r="O80" s="15"/>
+      <c r="N80" s="15" t="s">
+        <v>866</v>
+      </c>
+      <c r="O80" s="15" t="s">
+        <v>840</v>
+      </c>
       <c r="P80" s="21" t="s">
-        <v>870</v>
+        <v>902</v>
       </c>
       <c r="Q80" s="15"/>
       <c r="R80" s="15"/>
@@ -17104,10 +17246,14 @@
       <c r="M81" s="15" t="s">
         <v>714</v>
       </c>
-      <c r="N81" s="15"/>
-      <c r="O81" s="15"/>
+      <c r="N81" s="15" t="s">
+        <v>866</v>
+      </c>
+      <c r="O81" s="15" t="s">
+        <v>840</v>
+      </c>
       <c r="P81" s="15" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="Q81" s="15"/>
       <c r="R81" s="15"/>
@@ -17147,16 +17293,20 @@
       <c r="M82" s="15" t="s">
         <v>715</v>
       </c>
-      <c r="N82" s="15"/>
-      <c r="O82" s="15"/>
+      <c r="N82" s="15" t="s">
+        <v>866</v>
+      </c>
+      <c r="O82" s="15" t="s">
+        <v>840</v>
+      </c>
       <c r="P82" s="15" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="Q82" s="15"/>
       <c r="R82" s="15"/>
       <c r="S82" s="15"/>
       <c r="T82" s="51" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="U82" s="80"/>
     </row>
@@ -17191,7 +17341,7 @@
       <c r="N83" s="15"/>
       <c r="O83" s="15"/>
       <c r="P83" s="21" t="s">
-        <v>874</v>
+        <v>903</v>
       </c>
       <c r="Q83" s="15"/>
       <c r="R83" s="15"/>
@@ -17234,7 +17384,7 @@
       <c r="N84" s="15"/>
       <c r="O84" s="15"/>
       <c r="P84" s="21" t="s">
-        <v>874</v>
+        <v>904</v>
       </c>
       <c r="Q84" s="15"/>
       <c r="R84" s="15"/>
@@ -17275,7 +17425,7 @@
       <c r="N85" s="15"/>
       <c r="O85" s="15"/>
       <c r="P85" s="21" t="s">
-        <v>874</v>
+        <v>905</v>
       </c>
       <c r="Q85" s="15"/>
       <c r="R85" s="15"/>
@@ -17316,7 +17466,7 @@
       <c r="N86" s="15"/>
       <c r="O86" s="15"/>
       <c r="P86" s="21" t="s">
-        <v>874</v>
+        <v>904</v>
       </c>
       <c r="Q86" s="15"/>
       <c r="R86" s="15"/>
@@ -17357,7 +17507,7 @@
       <c r="N87" s="15"/>
       <c r="O87" s="15"/>
       <c r="P87" s="21" t="s">
-        <v>874</v>
+        <v>904</v>
       </c>
       <c r="Q87" s="15"/>
       <c r="R87" s="15"/>
@@ -17395,10 +17545,14 @@
       </c>
       <c r="L88" s="15"/>
       <c r="M88" s="21"/>
-      <c r="N88" s="15"/>
-      <c r="O88" s="15"/>
+      <c r="N88" s="15" t="s">
+        <v>866</v>
+      </c>
+      <c r="O88" s="15" t="s">
+        <v>840</v>
+      </c>
       <c r="P88" s="15" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="Q88" s="15"/>
       <c r="R88" s="15"/>
@@ -17445,7 +17599,7 @@
       <c r="N89" s="15"/>
       <c r="O89" s="15"/>
       <c r="P89" s="15" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="Q89" s="15"/>
       <c r="R89" s="15"/>
@@ -17492,7 +17646,7 @@
       <c r="N90" s="15"/>
       <c r="O90" s="15"/>
       <c r="P90" s="15" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="Q90" s="15"/>
       <c r="R90" s="15"/>
@@ -17535,7 +17689,7 @@
       <c r="N91" s="15"/>
       <c r="O91" s="15"/>
       <c r="P91" s="15" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="Q91" s="15"/>
       <c r="R91" s="15"/>
@@ -17543,7 +17697,7 @@
       <c r="T91" s="51"/>
       <c r="U91" s="80"/>
     </row>
-    <row r="92" spans="1:21" s="47" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:21" s="47" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A92" s="44">
         <v>91</v>
       </c>
@@ -17576,13 +17730,13 @@
         <v>716</v>
       </c>
       <c r="N92" s="15" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="O92" s="15" t="s">
         <v>840</v>
       </c>
       <c r="P92" s="15" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="Q92" s="15"/>
       <c r="R92" s="15"/>
@@ -17624,10 +17778,14 @@
       <c r="M93" s="15" t="s">
         <v>717</v>
       </c>
-      <c r="N93" s="15"/>
-      <c r="O93" s="15"/>
+      <c r="N93" s="15" t="s">
+        <v>876</v>
+      </c>
+      <c r="O93" s="15" t="s">
+        <v>840</v>
+      </c>
       <c r="P93" s="15" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="Q93" s="15"/>
       <c r="R93" s="15"/>
@@ -17669,10 +17827,14 @@
       <c r="M94" s="13" t="s">
         <v>806</v>
       </c>
-      <c r="N94" s="15"/>
-      <c r="O94" s="15"/>
+      <c r="N94" s="15" t="s">
+        <v>876</v>
+      </c>
+      <c r="O94" s="15" t="s">
+        <v>840</v>
+      </c>
       <c r="P94" s="15" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="Q94" s="15"/>
       <c r="R94" s="15"/>
@@ -17716,10 +17878,14 @@
       <c r="M95" s="15" t="s">
         <v>808</v>
       </c>
-      <c r="N95" s="15"/>
-      <c r="O95" s="15"/>
+      <c r="N95" s="15" t="s">
+        <v>876</v>
+      </c>
+      <c r="O95" s="15" t="s">
+        <v>840</v>
+      </c>
       <c r="P95" s="15" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="Q95" s="15"/>
       <c r="R95" s="15"/>
@@ -17759,10 +17925,14 @@
       <c r="M96" s="15" t="s">
         <v>718</v>
       </c>
-      <c r="N96" s="15"/>
-      <c r="O96" s="15"/>
+      <c r="N96" s="15" t="s">
+        <v>876</v>
+      </c>
+      <c r="O96" s="15" t="s">
+        <v>840</v>
+      </c>
       <c r="P96" s="15" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="Q96" s="15"/>
       <c r="R96" s="15"/>
@@ -17801,7 +17971,7 @@
       <c r="N97" s="15"/>
       <c r="O97" s="15"/>
       <c r="P97" s="21" t="s">
-        <v>874</v>
+        <v>903</v>
       </c>
       <c r="Q97" s="15"/>
       <c r="R97" s="15"/>
@@ -17844,7 +18014,7 @@
       <c r="N98" s="15"/>
       <c r="O98" s="15"/>
       <c r="P98" s="21" t="s">
-        <v>874</v>
+        <v>904</v>
       </c>
       <c r="Q98" s="15"/>
       <c r="R98" s="15"/>
@@ -17885,7 +18055,7 @@
       <c r="N99" s="15"/>
       <c r="O99" s="15"/>
       <c r="P99" s="21" t="s">
-        <v>874</v>
+        <v>905</v>
       </c>
       <c r="Q99" s="15"/>
       <c r="R99" s="15"/>
@@ -17926,7 +18096,7 @@
       <c r="N100" s="15"/>
       <c r="O100" s="15"/>
       <c r="P100" s="21" t="s">
-        <v>874</v>
+        <v>904</v>
       </c>
       <c r="Q100" s="15"/>
       <c r="R100" s="15"/>
@@ -17967,7 +18137,7 @@
       <c r="N101" s="15"/>
       <c r="O101" s="15"/>
       <c r="P101" s="21" t="s">
-        <v>874</v>
+        <v>904</v>
       </c>
       <c r="Q101" s="15"/>
       <c r="R101" s="15"/>
@@ -18010,7 +18180,7 @@
       <c r="N102" s="15"/>
       <c r="O102" s="15"/>
       <c r="P102" s="15" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="Q102" s="15"/>
       <c r="R102" s="15"/>
@@ -18053,7 +18223,7 @@
       <c r="N103" s="15"/>
       <c r="O103" s="15"/>
       <c r="P103" s="15" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="Q103" s="15"/>
       <c r="R103" s="15"/>
@@ -18094,7 +18264,7 @@
       <c r="N104" s="15"/>
       <c r="O104" s="15"/>
       <c r="P104" s="15" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="Q104" s="15"/>
       <c r="R104" s="15"/>
@@ -18135,7 +18305,7 @@
       <c r="N105" s="15"/>
       <c r="O105" s="15"/>
       <c r="P105" s="15" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="Q105" s="15"/>
       <c r="R105" s="15"/>
@@ -18178,7 +18348,7 @@
       <c r="N106" s="15"/>
       <c r="O106" s="15"/>
       <c r="P106" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="Q106" s="15"/>
       <c r="R106" s="15"/>
@@ -18186,7 +18356,7 @@
       <c r="T106" s="51"/>
       <c r="U106" s="80"/>
     </row>
-    <row r="107" spans="1:21" s="47" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:21" s="47" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A107" s="44">
         <v>106</v>
       </c>
@@ -18221,7 +18391,7 @@
       <c r="N107" s="15"/>
       <c r="O107" s="15"/>
       <c r="P107" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="Q107" s="15"/>
       <c r="R107" s="15"/>
@@ -18264,7 +18434,7 @@
       <c r="N108" s="15"/>
       <c r="O108" s="15"/>
       <c r="P108" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="Q108" s="15"/>
       <c r="R108" s="15"/>
@@ -18307,7 +18477,7 @@
       <c r="N109" s="15"/>
       <c r="O109" s="15"/>
       <c r="P109" s="15" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="Q109" s="15"/>
       <c r="R109" s="15"/>
@@ -33475,8 +33645,12 @@
       <sortCondition ref="A1:A478"/>
     </sortState>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="S10" r:id="rId1" display="https://www.hl7.org/fhir/us/core/StructureDefinition-us-core-race.html" xr:uid="{754BC80E-EC22-4F29-93B0-C379076F1467}"/>
+    <hyperlink ref="S11" r:id="rId2" display="https://www.hl7.org/fhir/us/core/StructureDefinition-us-core-ethnicity.html" xr:uid="{F9581B12-4613-4E92-BDA8-AB4E6E9762A1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>